<commit_message>
added now the original files without office back in
</commit_message>
<xml_diff>
--- a/Data_files/Rotterdam_car_adjacency_peri.xlsx
+++ b/Data_files/Rotterdam_car_adjacency_peri.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TimEW\PycharmProjects\Design_in_Network_group_8\Data_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2BE1FA0-D63B-44F9-BD89-35D9F28B0ECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BE4A692-91B1-4FEA-9BF4-66C445C5ACBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="12980" windowHeight="13770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -756,7 +756,7 @@
   <dimension ref="A1:U39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -843,7 +843,7 @@
         <v>106086</v>
       </c>
       <c r="E2" s="9">
-        <v>111.3943675892596</v>
+        <v>113.9789267</v>
       </c>
       <c r="F2" s="10">
         <v>0</v>
@@ -909,7 +909,7 @@
         <v>562839</v>
       </c>
       <c r="E3" s="13">
-        <v>591.0025305843493</v>
+        <v>604.71490226709398</v>
       </c>
       <c r="F3" s="3">
         <v>1</v>
@@ -975,7 +975,7 @@
         <v>121434</v>
       </c>
       <c r="E4" s="13">
-        <v>127.51035606804055</v>
+        <v>130.46883645572231</v>
       </c>
       <c r="F4" s="3">
         <v>0</v>
@@ -1041,7 +1041,7 @@
         <v>75316</v>
       </c>
       <c r="E5" s="13">
-        <v>79.084687794361898</v>
+        <v>80.919601483103435</v>
       </c>
       <c r="F5" s="3">
         <v>0</v>
@@ -1173,7 +1173,7 @@
         <v>110650</v>
       </c>
       <c r="E7" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F7" s="3">
         <v>0</v>
@@ -1239,7 +1239,7 @@
         <v>110650</v>
       </c>
       <c r="E8" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F8" s="3">
         <v>0</v>
@@ -1305,7 +1305,7 @@
         <v>110650</v>
       </c>
       <c r="E9" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F9" s="3">
         <v>0</v>
@@ -1371,7 +1371,7 @@
         <v>110650</v>
       </c>
       <c r="E10" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F10" s="3">
         <v>0</v>
@@ -1437,7 +1437,7 @@
         <v>110650</v>
       </c>
       <c r="E11" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F11" s="3">
         <v>0</v>
@@ -1503,7 +1503,7 @@
         <v>110650</v>
       </c>
       <c r="E12" s="13">
-        <v>116.18674258386183</v>
+        <v>118.88249381413505</v>
       </c>
       <c r="F12" s="3">
         <v>0</v>
@@ -1560,16 +1560,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="25">
-        <v>51.922169570000001</v>
+        <v>51.922169573927299</v>
       </c>
       <c r="C13" s="26">
-        <v>4.4098035900000001</v>
+        <v>4.4098035896042003</v>
       </c>
       <c r="D13" s="12">
         <v>77999</v>
       </c>
       <c r="E13" s="13">
-        <v>81.901940666955682</v>
+        <v>83.802219927778751</v>
       </c>
       <c r="F13" s="3">
         <v>1</v>
@@ -1635,7 +1635,7 @@
         <v>72561</v>
       </c>
       <c r="E14" s="13">
-        <v>76.191832161117077</v>
+        <v>77.959626151355195</v>
       </c>
       <c r="F14" s="3">
         <v>0</v>
@@ -1701,7 +1701,7 @@
         <v>75079</v>
       </c>
       <c r="E15" s="13">
-        <v>78.835828707218866</v>
+        <v>80.664968396488433</v>
       </c>
       <c r="F15" s="3">
         <v>0</v>
@@ -1767,7 +1767,7 @@
         <v>114887</v>
       </c>
       <c r="E16" s="13">
-        <v>120.63575504050739</v>
+        <v>123.43473173813405</v>
       </c>
       <c r="F16" s="3">
         <v>1</v>
@@ -1833,7 +1833,7 @@
         <v>126998</v>
       </c>
       <c r="E17" s="13">
-        <v>133.35276940501848</v>
+        <v>136.44680478452347</v>
       </c>
       <c r="F17" s="3">
         <v>0</v>
@@ -2000,6 +2000,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000967D3B9FC1DD84EB00B55E5790AB85E" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="92ec66a21d0d7142cf1fb1ae8fa08641">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="6ba023f1-a19b-4eec-904c-052d1f1cb5e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="62a86672aac255264bf3f3decc56659c" ns2:_="">
     <xsd:import namespace="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
@@ -2143,35 +2158,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2193,9 +2183,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4089522E-0C82-47E8-A49E-84CDA0FE73C2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{47226C14-663C-468E-81A1-C92460C7FBF2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6ba023f1-a19b-4eec-904c-052d1f1cb5e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>